<commit_message>
penambahan data lokasi pegawai
</commit_message>
<xml_diff>
--- a/assets/excel/Data Kota.xlsx
+++ b/assets/excel/Data Kota.xlsx
@@ -26,9 +26,6 @@
     <t>Malang</t>
   </si>
   <si>
-    <t>Nganjuk</t>
-  </si>
-  <si>
     <t>Blitar</t>
   </si>
   <si>
@@ -42,6 +39,9 @@
   </si>
   <si>
     <t>Paris</t>
+  </si>
+  <si>
+    <t>Cimahi</t>
   </si>
 </sst>
 </file>
@@ -406,7 +406,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -414,7 +414,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -422,7 +422,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -430,7 +430,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -438,7 +438,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -446,7 +446,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>

</xml_diff>